<commit_message>
updated fortress raid sheet export
</commit_message>
<xml_diff>
--- a/eden fortresss raid math updated.xlsx
+++ b/eden fortresss raid math updated.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>armySize</t>
   </si>
@@ -68,27 +68,30 @@
     <t>dead after armor</t>
   </si>
   <si>
+    <t>Roll / 50 if it didn't floor</t>
+  </si>
+  <si>
+    <t>soldier CR</t>
+  </si>
+  <si>
+    <t>max dead after clamp</t>
+  </si>
+  <si>
+    <t>final clamped dead</t>
+  </si>
+  <si>
     <t xml:space="preserve">actual damage </t>
   </si>
   <si>
-    <t>soldier CR</t>
-  </si>
-  <si>
-    <t>max dead after clamp</t>
-  </si>
-  <si>
-    <t>final clamped dead</t>
+    <t>min possible dead(base-max armor)</t>
+  </si>
+  <si>
+    <t>new remain best case</t>
   </si>
   <si>
     <t>average damage roll</t>
   </si>
   <si>
-    <t>min possible dead(base-max armor)</t>
-  </si>
-  <si>
-    <t>new remain best case</t>
-  </si>
-  <si>
     <t>max possible dead(base+max roll)</t>
   </si>
   <si>
@@ -101,13 +104,16 @@
     <t>troops max value</t>
   </si>
   <si>
-    <t>max damage</t>
+    <t>absolute max possible damage</t>
   </si>
   <si>
     <t>troops min value</t>
   </si>
   <si>
-    <t>min damage</t>
+    <t>worst case troops max damage</t>
+  </si>
+  <si>
+    <t>single remain max damage</t>
   </si>
   <si>
     <t>average armor benefit</t>
@@ -153,6 +159,9 @@
   </si>
   <si>
     <t xml:space="preserve">per armor probability divisor </t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
   <si>
     <t>base</t>
@@ -785,7 +794,7 @@
     <col customWidth="1" min="10" max="10" width="20.75"/>
     <col customWidth="1" min="11" max="11" width="11.38"/>
     <col customWidth="1" min="12" max="12" width="10.25"/>
-    <col customWidth="1" min="13" max="13" width="23.0"/>
+    <col customWidth="1" min="13" max="13" width="24.13"/>
     <col customWidth="1" min="14" max="14" width="14.25"/>
     <col customWidth="1" min="15" max="15" width="15.25"/>
     <col customWidth="1" min="16" max="17" width="16.0"/>
@@ -818,14 +827,14 @@
       </c>
       <c r="K1" s="2">
         <f>floor(RANDBETWEEN(0,H5),1)</f>
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="2">
         <f>B1-K9</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -857,14 +866,14 @@
       </c>
       <c r="K3" s="2">
         <f>H1+K1</f>
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="2">
         <f>N1*B9</f>
-        <v>2440</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -893,14 +902,14 @@
       </c>
       <c r="K5" s="2">
         <f>RANDBETWEEN(0,H7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="N5" s="2">
         <f>RANDBETWEEN(0,N3)</f>
-        <v>2056</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -922,15 +931,15 @@
       </c>
       <c r="K7" s="2">
         <f>K3-K5</f>
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="N7" s="2">
-        <f>FLOOR(N5/50,1)</f>
-        <v>41</v>
+        <f>N5/50</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -952,14 +961,14 @@
       </c>
       <c r="K9" s="2">
         <f>min(50, MAX(0, K7))</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="N9" s="2">
-        <f>FLOOR((N3/2)/50,1)</f>
-        <v>24</v>
+        <f>FLOOR(N5/50,1)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -982,10 +991,17 @@
         <f>B1-H11</f>
         <v>16</v>
       </c>
+      <c r="M11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="2">
+        <f>FLOOR((N3/2)/50,1)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H13" s="2">
         <f>H1+H5-0</f>
@@ -993,7 +1009,7 @@
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K13" s="2">
         <f>MAX(0,B1-H9)</f>
@@ -1002,21 +1018,21 @@
     </row>
     <row r="15">
       <c r="G15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H15" s="2">
         <f>E3-1</f>
         <v>12</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K15" s="2">
         <f>B9*K11</f>
         <v>3904</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N15" s="2">
         <f>FLOOR(K15/50,1)</f>
@@ -1025,23 +1041,32 @@
     </row>
     <row r="17">
       <c r="J17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K17" s="1">
         <f>K13*B9</f>
         <v>0</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N17" s="2">
         <f>FLOOR(K17/50,1)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="19">
+      <c r="M19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19" s="2">
+        <f>FLOOR(B9/50,1)</f>
+        <v>4</v>
+      </c>
+    </row>
     <row r="21">
       <c r="G21" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H21" s="2">
         <f>H7/2</f>
@@ -1050,14 +1075,14 @@
     </row>
     <row r="23">
       <c r="G23" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H23" s="2">
         <f>1/B7</f>
         <v>0.25</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N23" s="2">
         <f>FLOOR((B9/2)/50,1)</f>
@@ -1069,40 +1094,41 @@
     </row>
     <row r="25">
       <c r="G25" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H25" s="2">
         <f>E3+H21</f>
         <v>14.5</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K25" s="2">
         <f>(E3+H21)/(H3)</f>
         <v>0.3625</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="N25" s="1"/>
     </row>
     <row r="27">
       <c r="G27" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H27" s="2">
         <f>H25*(H25+1)</f>
         <v>224.75</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K27" s="2">
         <f>H27/H29</f>
         <v>2.809375</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N27" s="2">
         <f>K27*N23</f>
@@ -1111,7 +1137,7 @@
     </row>
     <row r="29">
       <c r="G29" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H29" s="2">
         <f>2*H3</f>
@@ -1120,14 +1146,14 @@
     </row>
     <row r="34">
       <c r="G34" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H34" s="2">
         <f>H21*B7</f>
         <v>6</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K34" s="2">
         <f>H38/H40</f>
@@ -1136,7 +1162,7 @@
     </row>
     <row r="36">
       <c r="G36" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H36" s="2">
         <f>(H15+1)*B7</f>
@@ -1145,7 +1171,7 @@
     </row>
     <row r="38">
       <c r="G38" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H38" s="2">
         <f>H36+H34</f>
@@ -1154,11 +1180,16 @@
     </row>
     <row r="40">
       <c r="G40" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H40" s="2">
         <f>(H3*B7)</f>
         <v>160</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="P41" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="50">
@@ -1223,7 +1254,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1">
         <v>1.0</v>
@@ -1231,7 +1262,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1">
         <v>12.0</v>
@@ -1241,34 +1272,34 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
@@ -1305,16 +1336,16 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
@@ -1345,7 +1376,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B5" s="13">
         <v>1.0</v>
@@ -1385,7 +1416,7 @@
     </row>
     <row r="6">
       <c r="A6" s="11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B6" s="15">
         <v>3.0</v>
@@ -1426,7 +1457,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="1"/>

</xml_diff>